<commit_message>
Simultaneous XYZ measurement, fix for groundLevelStable
Added bron event for simultaneous XYZ measurement (e.g. by GPS), i.e. a combination of BRO events
</commit_message>
<xml_diff>
--- a/BROMappings/Mapping BRO GMW Events.xlsx
+++ b/BROMappings/Mapping BRO GMW Events.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27231"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="28129"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://3hydro-my.sharepoint.com/personal/jos_von_asmuth_3hydro_nl/Documents/MATLAB/Menyanthes/Meny_OS/trunk/Datamodels/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://3hydro-my.sharepoint.com/personal/jos_von_asmuth_3hydro_nl/Documents/MATLAB/Menyanthes/Meny_OS/trunk/BronDatamodel/BROMappings/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="40" documentId="13_ncr:1_{7FA45A96-A3C0-4165-8D39-AC29C64859BA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{E20B8E9B-D637-4536-BA5B-A2E54CF0B9F4}"/>
+  <xr:revisionPtr revIDLastSave="41" documentId="13_ncr:1_{7FA45A96-A3C0-4165-8D39-AC29C64859BA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{CDD50771-71AE-4FF7-A0A7-48978A28285D}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="186" uniqueCount="100">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="199" uniqueCount="105">
   <si>
     <t>Put ingericht</t>
   </si>
@@ -325,6 +325,21 @@
   </si>
   <si>
     <t>Verwijdert individuele brondocumenten (aanvullingen, correcties, beëindiging). Het te verwijderen brondocument moet meegestuurd worden.</t>
+  </si>
+  <si>
+    <t>XYZPositie ingemeten</t>
+  </si>
+  <si>
+    <t>Aanvullen en corrigeren</t>
+  </si>
+  <si>
+    <t>Corrigeren (of geen)</t>
+  </si>
+  <si>
+    <t>Een nieuwe XY-inmeting hoeft niet noodzakelijkerwijs tot een correctie (verbeterde waarde) te leiden</t>
+  </si>
+  <si>
+    <t>Z en XY tegelijk ingemeten, combinatie van BRO-gebeurtenissen</t>
   </si>
 </sst>
 </file>
@@ -1122,10 +1137,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:G36"/>
+  <dimension ref="A1:G37"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="G30" sqref="G30"/>
+      <selection activeCell="G12" sqref="G12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1353,272 +1368,286 @@
       </c>
       <c r="G10" s="24"/>
     </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A11" s="2"/>
-      <c r="B11" s="14"/>
-      <c r="C11" s="14"/>
-      <c r="D11" s="14"/>
-      <c r="E11" s="30"/>
-      <c r="F11" s="38" t="s">
+    <row r="11" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+      <c r="A11" s="4" t="s">
+        <v>102</v>
+      </c>
+      <c r="B11" s="12" t="s">
+        <v>75</v>
+      </c>
+      <c r="C11" s="12" t="s">
+        <v>85</v>
+      </c>
+      <c r="D11" s="12" t="s">
+        <v>85</v>
+      </c>
+      <c r="E11" s="29" t="s">
+        <v>85</v>
+      </c>
+      <c r="F11" s="41" t="s">
         <v>46</v>
       </c>
-      <c r="G11" s="25"/>
+      <c r="G11" s="24" t="s">
+        <v>103</v>
+      </c>
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A12" s="4" t="s">
+      <c r="A12" s="2" t="s">
+        <v>101</v>
+      </c>
+      <c r="B12" s="14" t="s">
+        <v>10</v>
+      </c>
+      <c r="C12" s="14" t="s">
+        <v>10</v>
+      </c>
+      <c r="D12" s="14" t="s">
+        <v>10</v>
+      </c>
+      <c r="E12" s="30" t="s">
+        <v>10</v>
+      </c>
+      <c r="F12" s="38" t="s">
+        <v>100</v>
+      </c>
+      <c r="G12" s="25" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A13" s="4" t="s">
         <v>11</v>
       </c>
-      <c r="B12" s="12" t="s">
+      <c r="B13" s="12" t="s">
         <v>21</v>
       </c>
-      <c r="C12" s="12" t="s">
+      <c r="C13" s="12" t="s">
         <v>22</v>
       </c>
-      <c r="D12" s="12" t="s">
+      <c r="D13" s="12" t="s">
         <v>22</v>
       </c>
-      <c r="E12" s="29" t="s">
+      <c r="E13" s="29" t="s">
         <v>22</v>
       </c>
-      <c r="F12" s="31" t="s">
+      <c r="F13" s="31" t="s">
         <v>23</v>
       </c>
-      <c r="G12" s="24"/>
-    </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A13" s="2" t="s">
+      <c r="G13" s="24"/>
+    </row>
+    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A14" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="B13" s="14" t="s">
+      <c r="B14" s="14" t="s">
         <v>24</v>
       </c>
-      <c r="C13" s="14" t="s">
+      <c r="C14" s="14" t="s">
         <v>25</v>
       </c>
-      <c r="D13" s="14" t="s">
+      <c r="D14" s="14" t="s">
         <v>25</v>
       </c>
-      <c r="E13" s="30" t="s">
+      <c r="E14" s="30" t="s">
         <v>25</v>
       </c>
-      <c r="F13" s="38" t="s">
+      <c r="F14" s="38" t="s">
         <v>26</v>
       </c>
-      <c r="G13" s="25"/>
-    </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A14" s="3" t="s">
+      <c r="G14" s="25"/>
+    </row>
+    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A15" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="B14" s="13" t="s">
+      <c r="B15" s="13" t="s">
         <v>12</v>
       </c>
-      <c r="C14" s="13" t="s">
+      <c r="C15" s="13" t="s">
         <v>13</v>
       </c>
-      <c r="D14" s="13" t="s">
+      <c r="D15" s="13" t="s">
         <v>13</v>
       </c>
-      <c r="E14" s="35" t="s">
+      <c r="E15" s="35" t="s">
         <v>13</v>
       </c>
-      <c r="F14" s="40" t="s">
+      <c r="F15" s="40" t="s">
         <v>14</v>
       </c>
-      <c r="G14" s="24"/>
-    </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A15" s="4" t="s">
+      <c r="G15" s="24"/>
+    </row>
+    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A16" s="4" t="s">
         <v>11</v>
       </c>
-      <c r="B15" s="12" t="s">
+      <c r="B16" s="12" t="s">
         <v>15</v>
       </c>
-      <c r="C15" s="12" t="s">
+      <c r="C16" s="12" t="s">
         <v>16</v>
       </c>
-      <c r="D15" s="12" t="s">
+      <c r="D16" s="12" t="s">
         <v>16</v>
       </c>
-      <c r="E15" s="29" t="s">
+      <c r="E16" s="29" t="s">
         <v>16</v>
       </c>
-      <c r="F15" s="31" t="s">
+      <c r="F16" s="31" t="s">
         <v>17</v>
       </c>
-      <c r="G15" s="24"/>
-    </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A16" s="2" t="s">
+      <c r="G16" s="24"/>
+    </row>
+    <row r="17" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A17" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="B16" s="14" t="s">
+      <c r="B17" s="14" t="s">
         <v>18</v>
       </c>
-      <c r="C16" s="14" t="s">
+      <c r="C17" s="14" t="s">
         <v>19</v>
       </c>
-      <c r="D16" s="14" t="s">
+      <c r="D17" s="14" t="s">
         <v>19</v>
       </c>
-      <c r="E16" s="30" t="s">
+      <c r="E17" s="30" t="s">
         <v>19</v>
       </c>
-      <c r="F16" s="38" t="s">
+      <c r="F17" s="38" t="s">
         <v>20</v>
       </c>
-      <c r="G16" s="25"/>
-    </row>
-    <row r="17" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A17" s="4" t="s">
-        <v>11</v>
-      </c>
-      <c r="B17" s="12" t="s">
-        <v>48</v>
-      </c>
-      <c r="C17" s="12" t="s">
-        <v>49</v>
-      </c>
-      <c r="D17" s="12" t="s">
-        <v>49</v>
-      </c>
-      <c r="E17" s="29" t="s">
-        <v>49</v>
-      </c>
-      <c r="F17" s="31" t="s">
-        <v>50</v>
-      </c>
-      <c r="G17" s="24"/>
+      <c r="G17" s="25"/>
     </row>
     <row r="18" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A18" s="4" t="s">
         <v>11</v>
       </c>
       <c r="B18" s="12" t="s">
-        <v>51</v>
+        <v>48</v>
       </c>
       <c r="C18" s="12" t="s">
-        <v>52</v>
+        <v>49</v>
       </c>
       <c r="D18" s="12" t="s">
-        <v>52</v>
+        <v>49</v>
       </c>
       <c r="E18" s="29" t="s">
-        <v>52</v>
+        <v>49</v>
       </c>
       <c r="F18" s="31" t="s">
-        <v>53</v>
+        <v>50</v>
       </c>
       <c r="G18" s="24"/>
     </row>
-    <row r="19" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A19" s="4" t="s">
         <v>11</v>
       </c>
       <c r="B19" s="12" t="s">
+        <v>51</v>
+      </c>
+      <c r="C19" s="12" t="s">
+        <v>52</v>
+      </c>
+      <c r="D19" s="12" t="s">
+        <v>52</v>
+      </c>
+      <c r="E19" s="29" t="s">
+        <v>52</v>
+      </c>
+      <c r="F19" s="31" t="s">
+        <v>53</v>
+      </c>
+      <c r="G19" s="24"/>
+    </row>
+    <row r="20" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A20" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="B20" s="12" t="s">
         <v>96</v>
       </c>
-      <c r="C19" s="12" t="s">
+      <c r="C20" s="12" t="s">
         <v>95</v>
       </c>
-      <c r="D19" s="12" t="s">
+      <c r="D20" s="12" t="s">
         <v>95</v>
       </c>
-      <c r="E19" s="29" t="s">
+      <c r="E20" s="29" t="s">
         <v>95</v>
       </c>
-      <c r="F19" s="31" t="s">
+      <c r="F20" s="31" t="s">
         <v>94</v>
       </c>
-      <c r="G19" s="24" t="s">
+      <c r="G20" s="24" t="s">
         <v>97</v>
       </c>
     </row>
-    <row r="20" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A20" s="2" t="s">
+    <row r="21" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A21" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="B20" s="14" t="s">
+      <c r="B21" s="14" t="s">
         <v>54</v>
       </c>
-      <c r="C20" s="14" t="s">
+      <c r="C21" s="14" t="s">
         <v>55</v>
       </c>
-      <c r="D20" s="14" t="s">
+      <c r="D21" s="14" t="s">
         <v>55</v>
       </c>
-      <c r="E20" s="30" t="s">
+      <c r="E21" s="30" t="s">
         <v>55</v>
       </c>
-      <c r="F20" s="38" t="s">
+      <c r="F21" s="38" t="s">
         <v>56</v>
       </c>
-      <c r="G20" s="25"/>
-    </row>
-    <row r="21" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A21" s="4" t="s">
+      <c r="G21" s="25"/>
+    </row>
+    <row r="22" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A22" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="B21" s="12" t="s">
+      <c r="B22" s="12" t="s">
         <v>6</v>
       </c>
-      <c r="C21" s="12" t="s">
+      <c r="C22" s="12" t="s">
         <v>7</v>
       </c>
-      <c r="D21" s="12" t="s">
+      <c r="D22" s="12" t="s">
         <v>7</v>
       </c>
-      <c r="E21" s="29" t="s">
+      <c r="E22" s="29" t="s">
         <v>7</v>
       </c>
-      <c r="F21" s="31" t="s">
+      <c r="F22" s="31" t="s">
         <v>4</v>
       </c>
-      <c r="G21" s="24"/>
-    </row>
-    <row r="22" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A22" s="4" t="s">
+      <c r="G22" s="24"/>
+    </row>
+    <row r="23" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A23" s="4" t="s">
         <v>92</v>
       </c>
-      <c r="B22" s="12" t="s">
+      <c r="B23" s="12" t="s">
         <v>91</v>
       </c>
-      <c r="C22" s="12" t="s">
+      <c r="C23" s="12" t="s">
         <v>98</v>
       </c>
-      <c r="D22" s="12" t="s">
+      <c r="D23" s="12" t="s">
         <v>98</v>
       </c>
-      <c r="E22" s="12" t="s">
+      <c r="E23" s="12" t="s">
         <v>98</v>
       </c>
-      <c r="F22" s="31" t="s">
+      <c r="F23" s="31" t="s">
         <v>93</v>
       </c>
-      <c r="G22" s="24" t="s">
+      <c r="G23" s="24" t="s">
         <v>97</v>
       </c>
-    </row>
-    <row r="23" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A23" s="4" t="s">
-        <v>9</v>
-      </c>
-      <c r="B23" s="12" t="s">
-        <v>10</v>
-      </c>
-      <c r="C23" s="12" t="s">
-        <v>10</v>
-      </c>
-      <c r="D23" s="12" t="s">
-        <v>10</v>
-      </c>
-      <c r="E23" s="29" t="s">
-        <v>10</v>
-      </c>
-      <c r="F23" s="31" t="s">
-        <v>74</v>
-      </c>
-      <c r="G23" s="24"/>
     </row>
     <row r="24" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A24" s="4" t="s">
@@ -1637,7 +1666,7 @@
         <v>10</v>
       </c>
       <c r="F24" s="31" t="s">
-        <v>89</v>
+        <v>74</v>
       </c>
       <c r="G24" s="24"/>
     </row>
@@ -1658,70 +1687,70 @@
         <v>10</v>
       </c>
       <c r="F25" s="31" t="s">
+        <v>89</v>
+      </c>
+      <c r="G25" s="24"/>
+    </row>
+    <row r="26" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A26" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="B26" s="12" t="s">
+        <v>10</v>
+      </c>
+      <c r="C26" s="12" t="s">
+        <v>10</v>
+      </c>
+      <c r="D26" s="12" t="s">
+        <v>10</v>
+      </c>
+      <c r="E26" s="29" t="s">
+        <v>10</v>
+      </c>
+      <c r="F26" s="31" t="s">
         <v>8</v>
       </c>
-      <c r="G25" s="24"/>
-    </row>
-    <row r="26" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A26" s="8" t="s">
+      <c r="G26" s="24"/>
+    </row>
+    <row r="27" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A27" s="8" t="s">
         <v>9</v>
       </c>
-      <c r="B26" s="14" t="s">
-        <v>10</v>
-      </c>
-      <c r="C26" s="14" t="s">
-        <v>10</v>
-      </c>
-      <c r="D26" s="14" t="s">
-        <v>10</v>
-      </c>
-      <c r="E26" s="30" t="s">
-        <v>10</v>
-      </c>
-      <c r="F26" s="38" t="s">
+      <c r="B27" s="14" t="s">
+        <v>10</v>
+      </c>
+      <c r="C27" s="14" t="s">
+        <v>10</v>
+      </c>
+      <c r="D27" s="14" t="s">
+        <v>10</v>
+      </c>
+      <c r="E27" s="30" t="s">
+        <v>10</v>
+      </c>
+      <c r="F27" s="38" t="s">
         <v>90</v>
       </c>
-      <c r="G26" s="25"/>
-    </row>
-    <row r="27" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A27" s="3" t="s">
+      <c r="G27" s="25"/>
+    </row>
+    <row r="28" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A28" s="3" t="s">
         <v>47</v>
       </c>
-      <c r="B27" s="16" t="s">
+      <c r="B28" s="16" t="s">
         <v>76</v>
       </c>
-      <c r="C27" s="13" t="s">
+      <c r="C28" s="13" t="s">
         <v>84</v>
       </c>
-      <c r="D27" t="s">
+      <c r="D28" t="s">
         <v>84</v>
       </c>
-      <c r="E27" s="35" t="s">
+      <c r="E28" s="35" t="s">
         <v>84</v>
       </c>
-      <c r="F27" s="40" t="s">
+      <c r="F28" s="40" t="s">
         <v>79</v>
-      </c>
-      <c r="G27" s="24"/>
-    </row>
-    <row r="28" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A28" s="4" t="s">
-        <v>47</v>
-      </c>
-      <c r="B28" s="17" t="s">
-        <v>75</v>
-      </c>
-      <c r="C28" s="12" t="s">
-        <v>85</v>
-      </c>
-      <c r="D28" t="s">
-        <v>85</v>
-      </c>
-      <c r="E28" s="29" t="s">
-        <v>85</v>
-      </c>
-      <c r="F28" s="31" t="s">
-        <v>80</v>
       </c>
       <c r="G28" s="24"/>
     </row>
@@ -1730,55 +1759,65 @@
         <v>47</v>
       </c>
       <c r="B29" s="17" t="s">
+        <v>75</v>
+      </c>
+      <c r="C29" s="12" t="s">
+        <v>85</v>
+      </c>
+      <c r="D29" t="s">
+        <v>85</v>
+      </c>
+      <c r="E29" s="29" t="s">
+        <v>85</v>
+      </c>
+      <c r="F29" s="31" t="s">
+        <v>80</v>
+      </c>
+      <c r="G29" s="24"/>
+    </row>
+    <row r="30" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A30" s="4" t="s">
+        <v>47</v>
+      </c>
+      <c r="B30" s="17" t="s">
         <v>81</v>
       </c>
-      <c r="C29" s="12" t="s">
+      <c r="C30" s="12" t="s">
         <v>86</v>
       </c>
-      <c r="D29" t="s">
+      <c r="D30" t="s">
         <v>86</v>
       </c>
-      <c r="E29" s="29" t="s">
+      <c r="E30" s="29" t="s">
         <v>86</v>
       </c>
-      <c r="F29" s="31" t="s">
+      <c r="F30" s="31" t="s">
         <v>77</v>
       </c>
-      <c r="G29" s="24"/>
-    </row>
-    <row r="30" spans="1:7" ht="45" x14ac:dyDescent="0.25">
-      <c r="A30" s="2" t="s">
+      <c r="G30" s="24"/>
+    </row>
+    <row r="31" spans="1:7" ht="45" x14ac:dyDescent="0.25">
+      <c r="A31" s="2" t="s">
         <v>47</v>
       </c>
-      <c r="B30" s="18" t="s">
+      <c r="B31" s="18" t="s">
         <v>82</v>
       </c>
-      <c r="C30" s="14" t="s">
+      <c r="C31" s="14" t="s">
         <v>87</v>
       </c>
-      <c r="D30" s="21" t="s">
+      <c r="D31" s="21" t="s">
         <v>87</v>
       </c>
-      <c r="E30" s="30" t="s">
+      <c r="E31" s="30" t="s">
         <v>87</v>
       </c>
-      <c r="F30" s="38" t="s">
+      <c r="F31" s="38" t="s">
         <v>78</v>
       </c>
-      <c r="G30" s="25" t="s">
+      <c r="G31" s="25" t="s">
         <v>99</v>
       </c>
-    </row>
-    <row r="31" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A31" s="4"/>
-      <c r="B31" s="12"/>
-      <c r="C31" s="12"/>
-      <c r="D31" s="12"/>
-      <c r="E31" s="29"/>
-      <c r="F31" s="31" t="s">
-        <v>57</v>
-      </c>
-      <c r="G31" s="24"/>
     </row>
     <row r="32" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A32" s="4"/>
@@ -1787,7 +1826,7 @@
       <c r="D32" s="12"/>
       <c r="E32" s="29"/>
       <c r="F32" s="31" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="G32" s="24"/>
     </row>
@@ -1798,7 +1837,7 @@
       <c r="D33" s="12"/>
       <c r="E33" s="29"/>
       <c r="F33" s="31" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="G33" s="24"/>
     </row>
@@ -1809,7 +1848,7 @@
       <c r="D34" s="12"/>
       <c r="E34" s="29"/>
       <c r="F34" s="31" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="G34" s="24"/>
     </row>
@@ -1820,20 +1859,31 @@
       <c r="D35" s="12"/>
       <c r="E35" s="29"/>
       <c r="F35" s="31" t="s">
+        <v>60</v>
+      </c>
+      <c r="G35" s="24"/>
+    </row>
+    <row r="36" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A36" s="4"/>
+      <c r="B36" s="12"/>
+      <c r="C36" s="12"/>
+      <c r="D36" s="12"/>
+      <c r="E36" s="29"/>
+      <c r="F36" s="31" t="s">
         <v>61</v>
       </c>
-      <c r="G35" s="24"/>
-    </row>
-    <row r="36" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A36" s="9"/>
-      <c r="B36" s="19"/>
-      <c r="C36" s="19"/>
-      <c r="D36" s="19"/>
-      <c r="E36" s="36"/>
-      <c r="F36" s="32" t="s">
+      <c r="G36" s="24"/>
+    </row>
+    <row r="37" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A37" s="9"/>
+      <c r="B37" s="19"/>
+      <c r="C37" s="19"/>
+      <c r="D37" s="19"/>
+      <c r="E37" s="36"/>
+      <c r="F37" s="32" t="s">
         <v>62</v>
       </c>
-      <c r="G36" s="27"/>
+      <c r="G37" s="27"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>